<commit_message>
csv looking like a csv...
</commit_message>
<xml_diff>
--- a/Complete data/field_track.xlsx
+++ b/Complete data/field_track.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Il mio Drive\Spoke 7\Dati_Amelia\R\Complete data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE065E4-E3DC-4F07-96C3-4A09672552A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B208252A-4FA3-48BD-B429-81E76D8AB701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A8F51487-B761-4501-89D9-D9F813BCE4E6}"/>
   </bookViews>
@@ -1062,9 +1062,6 @@
     <t>Number of school buildings in a municipality</t>
   </si>
   <si>
-    <t>School order: primary, middle or high</t>
-  </si>
-  <si>
     <t>Proportion of school buildings provided with other heating systems</t>
   </si>
   <si>
@@ -1086,9 +1083,6 @@
     <t>Proportion of school buildings reached by private transport</t>
   </si>
   <si>
-    <t>Proportion of school buildings protected according to the Cultural Heritage Code, i.e. Legislative Decree 22/01/2004 n. 42 (ex Law 1089/39)</t>
-  </si>
-  <si>
     <t>Official statistical NUTS-3 code</t>
   </si>
   <si>
@@ -1179,24 +1173,6 @@
     <t>Proportion of school buildings whose doors are wide enough for wheelchair passage</t>
   </si>
   <si>
-    <t>Municipality classified as infrastructural pole, i.e. it is provided with a self-sufficient endowment in education, school and railway infrastructure (ISTAT inner areas taxonomy)</t>
-  </si>
-  <si>
-    <t>Municipality classified as inter-municipality infrastructural pole, i.e. belonging to a cluster of neighbouring municipality which taken together account for an infrastructural pole (ISTAT inner areas taxonomy)</t>
-  </si>
-  <si>
-    <t>Municipality classified as belt area, i.e. lying within a road travel time of about 27 minutes from the closest infrastructural pole (ISTAT inner areas taxonomy)</t>
-  </si>
-  <si>
-    <t>Municipality classified as intermediate inner area, i.e. lying within a road-travel distance of 27-40 minutes from the closest infrastructural pole (ISTAT inner areas taxonomy)</t>
-  </si>
-  <si>
-    <t>Municipality classified as peripheral inner area, i.e. lying within a road-travel distance of 40-66 minutes from the closest infrastructural pole (ISTAT inner areas taxonomy)</t>
-  </si>
-  <si>
-    <t>Municipality classified as ultra-peripheral inner area, i.e. lying within a road-travel distance greater than 66 minutes from the closest infrastructural pole (ISTAT inner areas taxonomy)</t>
-  </si>
-  <si>
     <t>Evacuation_plan</t>
   </si>
   <si>
@@ -1218,9 +1194,6 @@
     <t>Fire_prevention_certification</t>
   </si>
   <si>
-    <t>Proportion of school buildings with a fire prevention certificate - in Italian CPI, Certificato Prevenzione Incendi</t>
-  </si>
-  <si>
     <t>Fire_prevention_certification_MP</t>
   </si>
   <si>
@@ -1245,9 +1218,6 @@
     <t>Risk_assessment_document</t>
   </si>
   <si>
-    <t>Proportion of school buildings for which the risk assessment document has been produced - in Italian, DVR - Documento di Valutazione Rischi</t>
-  </si>
-  <si>
     <t>Risk_assessment_document_MP</t>
   </si>
   <si>
@@ -1258,6 +1228,36 @@
   </si>
   <si>
     <t>Thermal_plant_INAIL_certification_booklet_MP</t>
+  </si>
+  <si>
+    <t>Municipality classified as infrastructural pole - i.e. it is provided with a self-sufficient endowment in education school and railway infrastructure (ISTAT inner areas taxonomy)</t>
+  </si>
+  <si>
+    <t>Municipality classified as inter-municipality infrastructural pole - i.e. belonging to a cluster of neighbouring municipality which taken together account for an infrastructural pole (ISTAT inner areas taxonomy)</t>
+  </si>
+  <si>
+    <t>Municipality classified as belt area - i.e. lying within a road travel time of about 27 minutes from the closest infrastructural pole (ISTAT inner areas taxonomy)</t>
+  </si>
+  <si>
+    <t>Municipality classified as intermediate inner area - i.e. lying within a road-travel distance of 27-40 minutes from the closest infrastructural pole (ISTAT inner areas taxonomy)</t>
+  </si>
+  <si>
+    <t>Municipality classified as peripheral inner area - i.e. lying within a road-travel distance of 40-66 minutes from the closest infrastructural pole (ISTAT inner areas taxonomy)</t>
+  </si>
+  <si>
+    <t>Municipality classified as ultra-peripheral inner area - i.e. lying within a road-travel distance greater than 66 minutes from the closest infrastructural pole (ISTAT inner areas taxonomy)</t>
+  </si>
+  <si>
+    <t>School order: primary - middle or high</t>
+  </si>
+  <si>
+    <t>Proportion of school buildings protected according to the Cultural Heritage Code - i.e. Legislative Decree 22/01/2004 n. 42 (ex Law 1089/39)</t>
+  </si>
+  <si>
+    <t>Proportion of school buildings with a fire prevention certificate - in Italian CPI: Certificato Prevenzione Incendi</t>
+  </si>
+  <si>
+    <t>Proportion of school buildings for which the risk assessment document has been produced - in Italian: DVR - Documento di Valutazione Rischi</t>
   </si>
 </sst>
 </file>
@@ -1759,8 +1759,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2118,8 +2118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{607A3DCA-192C-42DB-8E11-F0A6FABCEFF8}">
   <dimension ref="A1:B292"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A270" workbookViewId="0">
-      <selection activeCell="A270" sqref="A1:B1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A271" workbookViewId="0">
+      <selection activeCell="B289" sqref="B289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2141,7 +2141,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>381</v>
+        <v>398</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2341,7 +2341,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>382</v>
+        <v>399</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -2541,7 +2541,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>383</v>
+        <v>400</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -2805,7 +2805,7 @@
         <v>83</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>384</v>
+        <v>401</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
@@ -2949,7 +2949,7 @@
         <v>101</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>385</v>
+        <v>402</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
@@ -3045,7 +3045,7 @@
         <v>113</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>386</v>
+        <v>403</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
@@ -3501,7 +3501,7 @@
         <v>170</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>342</v>
+        <v>404</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
@@ -3509,7 +3509,7 @@
         <v>171</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
@@ -3525,7 +3525,7 @@
         <v>173</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
@@ -3541,7 +3541,7 @@
         <v>175</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
@@ -3557,7 +3557,7 @@
         <v>177</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.3">
@@ -3573,7 +3573,7 @@
         <v>179</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
@@ -3589,7 +3589,7 @@
         <v>181</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
@@ -3605,7 +3605,7 @@
         <v>183</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
@@ -3621,7 +3621,7 @@
         <v>185</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>350</v>
+        <v>405</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
@@ -3637,7 +3637,7 @@
         <v>187</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
@@ -3645,7 +3645,7 @@
         <v>188</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
@@ -3653,7 +3653,7 @@
         <v>189</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
@@ -3669,7 +3669,7 @@
         <v>191</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
@@ -3685,7 +3685,7 @@
         <v>193</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
@@ -3693,7 +3693,7 @@
         <v>194</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
@@ -3701,7 +3701,7 @@
         <v>195</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
@@ -3709,7 +3709,7 @@
         <v>196</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
@@ -3717,7 +3717,7 @@
         <v>197</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
@@ -3725,7 +3725,7 @@
         <v>198</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
@@ -3733,7 +3733,7 @@
         <v>199</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
@@ -3741,7 +3741,7 @@
         <v>200</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
@@ -3749,7 +3749,7 @@
         <v>201</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
@@ -3757,7 +3757,7 @@
         <v>202</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
@@ -3765,7 +3765,7 @@
         <v>203</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.3">
@@ -3773,7 +3773,7 @@
         <v>204</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
@@ -3781,7 +3781,7 @@
         <v>205</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
@@ -3789,7 +3789,7 @@
         <v>206</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
@@ -3797,7 +3797,7 @@
         <v>207</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.3">
@@ -3805,7 +3805,7 @@
         <v>208</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.3">
@@ -3813,7 +3813,7 @@
         <v>209</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.3">
@@ -3829,7 +3829,7 @@
         <v>211</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
@@ -3845,7 +3845,7 @@
         <v>213</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
@@ -3861,7 +3861,7 @@
         <v>215</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
@@ -3877,7 +3877,7 @@
         <v>217</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
@@ -3893,7 +3893,7 @@
         <v>219</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.3">
@@ -3909,7 +3909,7 @@
         <v>221</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
@@ -3925,7 +3925,7 @@
         <v>223</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
@@ -3941,7 +3941,7 @@
         <v>225</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.3">
@@ -3957,7 +3957,7 @@
         <v>227</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
@@ -3973,7 +3973,7 @@
         <v>229</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
@@ -3981,7 +3981,7 @@
         <v>230</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
@@ -3989,7 +3989,7 @@
         <v>231</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.3">
@@ -3997,7 +3997,7 @@
         <v>232</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.3">
@@ -4005,7 +4005,7 @@
         <v>233</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.3">
@@ -4013,7 +4013,7 @@
         <v>234</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
@@ -4021,7 +4021,7 @@
         <v>235</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
@@ -4029,7 +4029,7 @@
         <v>236</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
@@ -4037,7 +4037,7 @@
         <v>237</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.3">
@@ -4045,7 +4045,7 @@
         <v>238</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
@@ -4053,7 +4053,7 @@
         <v>239</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.3">
@@ -4061,7 +4061,7 @@
         <v>240</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.3">
@@ -4069,7 +4069,7 @@
         <v>241</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.3">
@@ -4077,7 +4077,7 @@
         <v>242</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
@@ -4085,7 +4085,7 @@
         <v>243</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.3">
@@ -4093,7 +4093,7 @@
         <v>244</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
@@ -4101,7 +4101,7 @@
         <v>245</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
@@ -4109,7 +4109,7 @@
         <v>246</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
@@ -4117,7 +4117,7 @@
         <v>247</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
@@ -4125,7 +4125,7 @@
         <v>248</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
@@ -4133,7 +4133,7 @@
         <v>249</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
@@ -4141,7 +4141,7 @@
         <v>250</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.3">
@@ -4149,7 +4149,7 @@
         <v>251</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
@@ -4157,7 +4157,7 @@
         <v>252</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.3">
@@ -4165,7 +4165,7 @@
         <v>253</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.3">
@@ -4173,7 +4173,7 @@
         <v>254</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.3">
@@ -4181,7 +4181,7 @@
         <v>255</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.3">
@@ -4189,7 +4189,7 @@
         <v>256</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.3">
@@ -4205,7 +4205,7 @@
         <v>258</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.3">
@@ -4213,7 +4213,7 @@
         <v>259</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.3">
@@ -4221,7 +4221,7 @@
         <v>260</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.3">
@@ -4237,7 +4237,7 @@
         <v>262</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.3">
@@ -4253,7 +4253,7 @@
         <v>264</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.3">
@@ -4261,7 +4261,7 @@
         <v>265</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.3">
@@ -4269,7 +4269,7 @@
         <v>266</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.3">
@@ -4277,7 +4277,7 @@
         <v>267</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.3">
@@ -4293,7 +4293,7 @@
         <v>269</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.3">
@@ -4309,7 +4309,7 @@
         <v>271</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.3">
@@ -4325,7 +4325,7 @@
         <v>273</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.3">
@@ -4341,7 +4341,7 @@
         <v>275</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.3">
@@ -4354,15 +4354,15 @@
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A279" s="3" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A280" s="3" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="B280" s="3" t="s">
         <v>279</v>
@@ -4370,15 +4370,15 @@
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A281" s="3" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A282" s="3" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="B282" s="3" t="s">
         <v>279</v>
@@ -4386,15 +4386,15 @@
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A283" s="3" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>394</v>
+        <v>406</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A284" s="3" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="B284" s="3" t="s">
         <v>279</v>
@@ -4402,15 +4402,15 @@
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A285" s="3" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A286" s="3" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="B286" s="3" t="s">
         <v>279</v>
@@ -4418,15 +4418,15 @@
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A287" s="3" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A288" s="3" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
       <c r="B288" s="3" t="s">
         <v>279</v>
@@ -4434,15 +4434,15 @@
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A289" s="3" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A290" s="3" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="B290" s="3" t="s">
         <v>279</v>
@@ -4450,15 +4450,15 @@
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A291" s="3" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A292" s="3" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="B292" s="3" t="s">
         <v>279</v>

</xml_diff>

<commit_message>
more informative fields descriptions for classroom size and invalsi
</commit_message>
<xml_diff>
--- a/Complete data/field_track.xlsx
+++ b/Complete data/field_track.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Il mio Drive\Spoke 7\Dati_Amelia\R\Complete data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B208252A-4FA3-48BD-B429-81E76D8AB701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E2DB21-8648-434F-9D41-0E4395B0B360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A8F51487-B761-4501-89D9-D9F813BCE4E6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="485">
   <si>
     <t>A_mun</t>
   </si>
@@ -924,9 +924,6 @@
     <t>Most frequent building period class of school buildings</t>
   </si>
   <si>
-    <t>Students coverage in Invalsi tests</t>
-  </si>
-  <si>
     <t>Proportion of school buildings with a school restaurant/canteen</t>
   </si>
   <si>
@@ -942,9 +939,6 @@
     <t>Proportion of school buildings provided with centralised methane heating systems</t>
   </si>
   <si>
-    <t>Average number of classrooms of the grade in scope per municipality</t>
-  </si>
-  <si>
     <t>Proportion of school buildings adequately provided with classrooms</t>
   </si>
   <si>
@@ -1047,9 +1041,6 @@
     <t>Proportion of schools not provided with an external layby</t>
   </si>
   <si>
-    <t>Average invalsi score of subject and school grade in scope</t>
-  </si>
-  <si>
     <t>Official statistical LAU code</t>
   </si>
   <si>
@@ -1095,9 +1086,6 @@
     <t>Proportion of school buildings lying close to train stations</t>
   </si>
   <si>
-    <t>Standard deviation of the Invalsi score of subject and grade in scope</t>
-  </si>
-  <si>
     <t>Proportion of school buildings with specific critical issues</t>
   </si>
   <si>
@@ -1128,9 +1116,6 @@
     <t>Proportion of school buildings which underwent static testing</t>
   </si>
   <si>
-    <t>Average number of students per school attending the grade in scope</t>
-  </si>
-  <si>
     <t>Average number of students</t>
   </si>
   <si>
@@ -1248,9 +1233,6 @@
     <t>Municipality classified as ultra-peripheral inner area - i.e. lying within a road-travel distance greater than 66 minutes from the closest infrastructural pole (ISTAT inner areas taxonomy)</t>
   </si>
   <si>
-    <t>School order: primary - middle or high</t>
-  </si>
-  <si>
     <t>Proportion of school buildings protected according to the Cultural Heritage Code - i.e. Legislative Decree 22/01/2004 n. 42 (ex Law 1089/39)</t>
   </si>
   <si>
@@ -1258,6 +1240,255 @@
   </si>
   <si>
     <t>Proportion of school buildings for which the risk assessment document has been produced - in Italian: DVR - Documento di Valutazione Rischi</t>
+  </si>
+  <si>
+    <t>Students coverage in Invalsi tests in English listening at the final year of high school</t>
+  </si>
+  <si>
+    <t>Students coverage in Invalsi tests in English listening at the final year of primary school</t>
+  </si>
+  <si>
+    <t>Students coverage in Invalsi tests in English listening at the final year of middle school</t>
+  </si>
+  <si>
+    <t>Students coverage in Invalsi tests in English reading at the final year of high school</t>
+  </si>
+  <si>
+    <t>Students coverage in Invalsi tests at the final year of primary school</t>
+  </si>
+  <si>
+    <t>Students coverage in Invalsi tests at the final year of middle school</t>
+  </si>
+  <si>
+    <t>Students coverage in Invalsi tests in Italian at the second year of high school</t>
+  </si>
+  <si>
+    <t>Students coverage in Invalsi tests in Italian at the final year of high school</t>
+  </si>
+  <si>
+    <t>Students coverage in Invalsi tests in Italian at the second year of primary school</t>
+  </si>
+  <si>
+    <t>Students coverage in Invalsi tests in Italian at the final year of primary school</t>
+  </si>
+  <si>
+    <t>Students coverage in Invalsi tests in Italian at the final year of middle school</t>
+  </si>
+  <si>
+    <t>Students coverage in Invalsi tests in Mathematics at the final year of middle school</t>
+  </si>
+  <si>
+    <t>Students coverage in Invalsi tests in Mathematics at the final year of high school</t>
+  </si>
+  <si>
+    <t>Students coverage in Invalsi tests in Mathematics at the second year of primary school</t>
+  </si>
+  <si>
+    <t>Students coverage in Invalsi tests in Mathematics at the final year of primary school</t>
+  </si>
+  <si>
+    <t>Average number of classrooms per municipality for the first year of primary school</t>
+  </si>
+  <si>
+    <t>Average number of classrooms per municipality for the second year of high school</t>
+  </si>
+  <si>
+    <t>Average number of classrooms per municipality for the third year of high school</t>
+  </si>
+  <si>
+    <t>Average number of classrooms per municipality for the fourth year of high school</t>
+  </si>
+  <si>
+    <t>Average number of classrooms per municipality for the final year of high school</t>
+  </si>
+  <si>
+    <t>Average number of classrooms per municipality for the second year of primary school</t>
+  </si>
+  <si>
+    <t>Average number of classrooms per municipality for the third year of primary school</t>
+  </si>
+  <si>
+    <t>Average number of classrooms per municipality for the fourth year of primary school</t>
+  </si>
+  <si>
+    <t>Average number of classrooms per municipality for the fifth year of primary school</t>
+  </si>
+  <si>
+    <t>Average number of classrooms per municipality for the first year of middle school</t>
+  </si>
+  <si>
+    <t>Average number of classrooms per municipality for the second year of middle school</t>
+  </si>
+  <si>
+    <t>Average number of classrooms per municipality for the final year of middle school</t>
+  </si>
+  <si>
+    <t>Average WLE Invalsi score in English listening at the final year of high school</t>
+  </si>
+  <si>
+    <t>Average WLE Invalsi score in English listening at the final year of primary school</t>
+  </si>
+  <si>
+    <t>Average WLE Invalsi score in English listening at the final year of middle school</t>
+  </si>
+  <si>
+    <t>Average WLE invalsi score in English reading at the final year of high school</t>
+  </si>
+  <si>
+    <t>Average WLE invalsi score in English reading at the final year of middle school</t>
+  </si>
+  <si>
+    <t>Average WLE invalsi score in English reading at the final year of primary school</t>
+  </si>
+  <si>
+    <t>Average WLE invalsi score in Italian at the second year of high school</t>
+  </si>
+  <si>
+    <t>Average WLE invalsi score in Italian at the final year of high school</t>
+  </si>
+  <si>
+    <t>Average WLE invalsi score in Italian at the second year of primary school</t>
+  </si>
+  <si>
+    <t>Average WLE invalsi score in Italian at the final year of primary school</t>
+  </si>
+  <si>
+    <t>Average WLE invalsi score in Italian at the final year of middle school</t>
+  </si>
+  <si>
+    <t>Average WLE invalsi score in Mathematics at the second year of high school</t>
+  </si>
+  <si>
+    <t>Average WLE invalsi score in Mathematics at the final year of high school</t>
+  </si>
+  <si>
+    <t>Average WLE invalsi score in Mathematics at the second year of primary school</t>
+  </si>
+  <si>
+    <t>Average WLE invalsi score in Mathematics at the final year of middle school</t>
+  </si>
+  <si>
+    <t>School order. either primary - middle - high - IC namely comprehensive institute - IS namely superior institute - or NR namely different school orders</t>
+  </si>
+  <si>
+    <t>Average number of students per school attending the first year of primary school</t>
+  </si>
+  <si>
+    <t>Average number of students per school attending the second year of high school</t>
+  </si>
+  <si>
+    <t>Average number of students per school attending the third year of high school</t>
+  </si>
+  <si>
+    <t>Average number of students per school attending the fourth year of high school</t>
+  </si>
+  <si>
+    <t>Average number of students per school attending the final year of high school</t>
+  </si>
+  <si>
+    <t>Average number of students per school attending the second year of primary school</t>
+  </si>
+  <si>
+    <t>Average number of students per school attending the third year of primary school</t>
+  </si>
+  <si>
+    <t>Average number of students per school attending the fourth year of primary school</t>
+  </si>
+  <si>
+    <t>Average number of students per school attending the final year of primary school</t>
+  </si>
+  <si>
+    <t>Average number of students per school attending the first year of middle school</t>
+  </si>
+  <si>
+    <t>Average number of students per school attending the final year of middle school</t>
+  </si>
+  <si>
+    <t>Average number of students per school attending the first year of high school</t>
+  </si>
+  <si>
+    <t>Average classroom size - i.e. students per classroom - at the first year of primary school</t>
+  </si>
+  <si>
+    <t>Average classroom size - i.e. students per classroom - at the second year of high school</t>
+  </si>
+  <si>
+    <t>Average classroom size - i.e. students per classroom - at the third year of high school</t>
+  </si>
+  <si>
+    <t>Average classroom size - i.e. students per classroom - at the fourth year of high school</t>
+  </si>
+  <si>
+    <t>Average classroom size - i.e. students per classroom - at the final year of high school</t>
+  </si>
+  <si>
+    <t>Average classroom size - i.e. students per classroom - at the second year of primary school</t>
+  </si>
+  <si>
+    <t>Average classroom size - i.e. students per classroom - at the third year of primary school</t>
+  </si>
+  <si>
+    <t>Average classroom size - i.e. students per classroom - at the fourth year of primary school</t>
+  </si>
+  <si>
+    <t>Average classroom size - i.e. students per classroom - at the final year of primary school</t>
+  </si>
+  <si>
+    <t>Average classroom size - i.e. students per classroom - at the first year of middle school</t>
+  </si>
+  <si>
+    <t>Average classroom size - i.e. students per classroom - at the final year of middle school</t>
+  </si>
+  <si>
+    <t>Average classroom size - i.e. students per classroom - at the first year of high school</t>
+  </si>
+  <si>
+    <t>Standard deviation of Invalsi WLE scores in English listening at the final year of high school</t>
+  </si>
+  <si>
+    <t>Standard deviation of Invalsi WLE scores in English listening at the final year of primary school</t>
+  </si>
+  <si>
+    <t>Standard deviation of Invalsi WLE scores in English listening at the final year of middle school</t>
+  </si>
+  <si>
+    <t>Standard deviation of Invalsi WLE scores in English reading at the final year of high school</t>
+  </si>
+  <si>
+    <t>Standard deviation of Invalsi WLE scores in English reading at the final year of primary school</t>
+  </si>
+  <si>
+    <t>Standard deviation of Invalsi WLE scores in English reading at the final year of middle school</t>
+  </si>
+  <si>
+    <t>Standard deviation of Invalsi WLE scores in Italian at the second year of high school</t>
+  </si>
+  <si>
+    <t>Standard deviation of Invalsi WLE scores in Italian at the final year of high school</t>
+  </si>
+  <si>
+    <t>Standard deviation of Invalsi WLE scores in Italian at the second year of primary school</t>
+  </si>
+  <si>
+    <t>Standard deviation of Invalsi WLE scores in Italian at the final year of primary school</t>
+  </si>
+  <si>
+    <t>Standard deviation of Invalsi WLE scores in Italian at the final year of middle school</t>
+  </si>
+  <si>
+    <t>Standard deviation of Invalsi WLE scores in Mathematics at the second year of high school</t>
+  </si>
+  <si>
+    <t>Standard deviation of Invalsi WLE scores in Mathematics at the final year of high school</t>
+  </si>
+  <si>
+    <t>Standard deviation of Invalsi WLE scores in Mathematics at the second year of primary school</t>
+  </si>
+  <si>
+    <t>Standard deviation of Invalsi WLE scores in Mathematics at the final year of primary school</t>
+  </si>
+  <si>
+    <t>Standard deviation of Invalsi WLE scores in Mathematics at the final year of middle school</t>
   </si>
 </sst>
 </file>
@@ -2118,8 +2349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{607A3DCA-192C-42DB-8E11-F0A6FABCEFF8}">
   <dimension ref="A1:B292"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A271" workbookViewId="0">
-      <selection activeCell="B289" sqref="B289"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2141,7 +2372,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2341,7 +2572,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -2413,7 +2644,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>296</v>
+        <v>402</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -2421,7 +2652,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>296</v>
+        <v>403</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -2429,7 +2660,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>296</v>
+        <v>404</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -2437,7 +2668,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>296</v>
+        <v>405</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -2445,7 +2676,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>296</v>
+        <v>406</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -2453,7 +2684,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>296</v>
+        <v>407</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -2461,7 +2692,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>296</v>
+        <v>408</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -2469,7 +2700,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>296</v>
+        <v>409</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -2477,7 +2708,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>296</v>
+        <v>410</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -2485,7 +2716,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>296</v>
+        <v>411</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -2493,7 +2724,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>296</v>
+        <v>412</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -2501,7 +2732,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>296</v>
+        <v>413</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -2509,7 +2740,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>296</v>
+        <v>414</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -2517,7 +2748,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>296</v>
+        <v>415</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -2525,7 +2756,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>296</v>
+        <v>416</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -2533,7 +2764,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>296</v>
+        <v>413</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -2541,7 +2772,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -2557,7 +2788,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -2573,7 +2804,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -2589,7 +2820,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -2605,7 +2836,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -2621,7 +2852,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
@@ -2637,7 +2868,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>302</v>
+        <v>417</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
@@ -2645,7 +2876,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>302</v>
+        <v>418</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
@@ -2653,7 +2884,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>302</v>
+        <v>419</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
@@ -2661,7 +2892,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>302</v>
+        <v>420</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
@@ -2669,7 +2900,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>302</v>
+        <v>421</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
@@ -2677,7 +2908,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>302</v>
+        <v>422</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
@@ -2685,7 +2916,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>302</v>
+        <v>423</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
@@ -2693,7 +2924,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>302</v>
+        <v>424</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
@@ -2701,7 +2932,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>302</v>
+        <v>425</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
@@ -2709,7 +2940,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>302</v>
+        <v>426</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
@@ -2717,7 +2948,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>302</v>
+        <v>427</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
@@ -2725,7 +2956,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>302</v>
+        <v>428</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
@@ -2733,7 +2964,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>302</v>
+        <v>417</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
@@ -2741,7 +2972,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
@@ -2757,7 +2988,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
@@ -2773,7 +3004,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
@@ -2789,7 +3020,7 @@
         <v>81</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
@@ -2805,7 +3036,7 @@
         <v>83</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
@@ -2821,7 +3052,7 @@
         <v>85</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
@@ -2837,7 +3068,7 @@
         <v>87</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
@@ -2853,7 +3084,7 @@
         <v>89</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
@@ -2869,7 +3100,7 @@
         <v>91</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
@@ -2885,7 +3116,7 @@
         <v>93</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
@@ -2901,7 +3132,7 @@
         <v>95</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
@@ -2917,7 +3148,7 @@
         <v>97</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
@@ -2933,7 +3164,7 @@
         <v>99</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
@@ -2949,7 +3180,7 @@
         <v>101</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
@@ -2965,7 +3196,7 @@
         <v>103</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
@@ -2981,7 +3212,7 @@
         <v>105</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
@@ -2997,7 +3228,7 @@
         <v>107</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
@@ -3013,7 +3244,7 @@
         <v>109</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
@@ -3029,7 +3260,7 @@
         <v>111</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
@@ -3045,7 +3276,7 @@
         <v>113</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
@@ -3061,7 +3292,7 @@
         <v>115</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
@@ -3077,7 +3308,7 @@
         <v>117</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
@@ -3093,7 +3324,7 @@
         <v>119</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
@@ -3109,7 +3340,7 @@
         <v>121</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
@@ -3125,7 +3356,7 @@
         <v>123</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
@@ -3141,7 +3372,7 @@
         <v>125</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
@@ -3157,7 +3388,7 @@
         <v>127</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
@@ -3173,7 +3404,7 @@
         <v>129</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
@@ -3189,7 +3420,7 @@
         <v>131</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
@@ -3205,7 +3436,7 @@
         <v>133</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
@@ -3221,7 +3452,7 @@
         <v>135</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
@@ -3237,7 +3468,7 @@
         <v>137</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
@@ -3253,7 +3484,7 @@
         <v>139</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
@@ -3269,7 +3500,7 @@
         <v>141</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
@@ -3285,7 +3516,7 @@
         <v>143</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
@@ -3301,7 +3532,7 @@
         <v>145</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
@@ -3317,7 +3548,7 @@
         <v>147</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
@@ -3333,7 +3564,7 @@
         <v>149</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>337</v>
+        <v>429</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
@@ -3341,7 +3572,7 @@
         <v>150</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>337</v>
+        <v>430</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
@@ -3349,7 +3580,7 @@
         <v>151</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>337</v>
+        <v>431</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
@@ -3357,7 +3588,7 @@
         <v>152</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>337</v>
+        <v>432</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
@@ -3365,7 +3596,7 @@
         <v>153</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>337</v>
+        <v>433</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
@@ -3373,7 +3604,7 @@
         <v>154</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>337</v>
+        <v>434</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
@@ -3381,7 +3612,7 @@
         <v>155</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>337</v>
+        <v>435</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
@@ -3389,7 +3620,7 @@
         <v>156</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>337</v>
+        <v>436</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
@@ -3397,7 +3628,7 @@
         <v>157</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>337</v>
+        <v>437</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
@@ -3405,7 +3636,7 @@
         <v>158</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>337</v>
+        <v>438</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
@@ -3413,7 +3644,7 @@
         <v>159</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>337</v>
+        <v>439</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
@@ -3421,7 +3652,7 @@
         <v>160</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>337</v>
+        <v>440</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
@@ -3429,7 +3660,7 @@
         <v>161</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>337</v>
+        <v>441</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
@@ -3437,7 +3668,7 @@
         <v>162</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>337</v>
+        <v>442</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
@@ -3445,7 +3676,7 @@
         <v>163</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>337</v>
+        <v>441</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
@@ -3453,7 +3684,7 @@
         <v>164</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>337</v>
+        <v>443</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
@@ -3461,7 +3692,7 @@
         <v>165</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
@@ -3469,7 +3700,7 @@
         <v>166</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
@@ -3477,7 +3708,7 @@
         <v>167</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
@@ -3493,7 +3724,7 @@
         <v>169</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
@@ -3501,7 +3732,7 @@
         <v>170</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>404</v>
+        <v>444</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
@@ -3509,7 +3740,7 @@
         <v>171</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
@@ -3525,7 +3756,7 @@
         <v>173</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
@@ -3541,7 +3772,7 @@
         <v>175</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
@@ -3557,7 +3788,7 @@
         <v>177</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.3">
@@ -3573,7 +3804,7 @@
         <v>179</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
@@ -3589,7 +3820,7 @@
         <v>181</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
@@ -3605,7 +3836,7 @@
         <v>183</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
@@ -3621,7 +3852,7 @@
         <v>185</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
@@ -3637,7 +3868,7 @@
         <v>187</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
@@ -3645,7 +3876,7 @@
         <v>188</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
@@ -3653,7 +3884,7 @@
         <v>189</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
@@ -3669,7 +3900,7 @@
         <v>191</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
@@ -3685,7 +3916,7 @@
         <v>193</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>353</v>
+        <v>469</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
@@ -3693,7 +3924,7 @@
         <v>194</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>353</v>
+        <v>470</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
@@ -3701,7 +3932,7 @@
         <v>195</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>353</v>
+        <v>471</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
@@ -3709,7 +3940,7 @@
         <v>196</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>353</v>
+        <v>472</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
@@ -3717,7 +3948,7 @@
         <v>197</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>353</v>
+        <v>473</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
@@ -3725,7 +3956,7 @@
         <v>198</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>353</v>
+        <v>474</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
@@ -3733,7 +3964,7 @@
         <v>199</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>353</v>
+        <v>475</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
@@ -3741,7 +3972,7 @@
         <v>200</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>353</v>
+        <v>476</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
@@ -3749,7 +3980,7 @@
         <v>201</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>353</v>
+        <v>477</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
@@ -3757,7 +3988,7 @@
         <v>202</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>353</v>
+        <v>478</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
@@ -3765,7 +3996,7 @@
         <v>203</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>353</v>
+        <v>479</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.3">
@@ -3773,7 +4004,7 @@
         <v>204</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>353</v>
+        <v>480</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
@@ -3781,7 +4012,7 @@
         <v>205</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>353</v>
+        <v>481</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
@@ -3789,7 +4020,7 @@
         <v>206</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>353</v>
+        <v>482</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
@@ -3797,7 +4028,7 @@
         <v>207</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>353</v>
+        <v>483</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.3">
@@ -3805,7 +4036,7 @@
         <v>208</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>353</v>
+        <v>484</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.3">
@@ -3813,7 +4044,7 @@
         <v>209</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.3">
@@ -3829,7 +4060,7 @@
         <v>211</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
@@ -3845,7 +4076,7 @@
         <v>213</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
@@ -3861,7 +4092,7 @@
         <v>215</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
@@ -3877,7 +4108,7 @@
         <v>217</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
@@ -3893,7 +4124,7 @@
         <v>219</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.3">
@@ -3909,7 +4140,7 @@
         <v>221</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
@@ -3925,7 +4156,7 @@
         <v>223</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
@@ -3941,7 +4172,7 @@
         <v>225</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.3">
@@ -3957,7 +4188,7 @@
         <v>227</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
@@ -3973,7 +4204,7 @@
         <v>229</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>364</v>
+        <v>445</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
@@ -3981,7 +4212,7 @@
         <v>230</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>364</v>
+        <v>446</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
@@ -3989,7 +4220,7 @@
         <v>231</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>364</v>
+        <v>447</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.3">
@@ -3997,7 +4228,7 @@
         <v>232</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>364</v>
+        <v>448</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.3">
@@ -4005,7 +4236,7 @@
         <v>233</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>364</v>
+        <v>449</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.3">
@@ -4013,7 +4244,7 @@
         <v>234</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>364</v>
+        <v>450</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
@@ -4021,7 +4252,7 @@
         <v>235</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>364</v>
+        <v>451</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
@@ -4029,7 +4260,7 @@
         <v>236</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>364</v>
+        <v>452</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
@@ -4037,7 +4268,7 @@
         <v>237</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>364</v>
+        <v>453</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.3">
@@ -4045,7 +4276,7 @@
         <v>238</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>364</v>
+        <v>454</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
@@ -4053,7 +4284,7 @@
         <v>239</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>364</v>
+        <v>450</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.3">
@@ -4061,7 +4292,7 @@
         <v>240</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>364</v>
+        <v>455</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.3">
@@ -4069,7 +4300,7 @@
         <v>241</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>364</v>
+        <v>456</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.3">
@@ -4077,7 +4308,7 @@
         <v>242</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>364</v>
+        <v>457</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
@@ -4085,7 +4316,7 @@
         <v>243</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>364</v>
+        <v>458</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.3">
@@ -4093,7 +4324,7 @@
         <v>244</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>364</v>
+        <v>459</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
@@ -4101,7 +4332,7 @@
         <v>245</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>364</v>
+        <v>460</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
@@ -4109,7 +4340,7 @@
         <v>246</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>364</v>
+        <v>461</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
@@ -4117,7 +4348,7 @@
         <v>247</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>364</v>
+        <v>462</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
@@ -4125,7 +4356,7 @@
         <v>248</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>364</v>
+        <v>463</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
@@ -4133,7 +4364,7 @@
         <v>249</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>364</v>
+        <v>464</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
@@ -4141,7 +4372,7 @@
         <v>250</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>364</v>
+        <v>465</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.3">
@@ -4149,7 +4380,7 @@
         <v>251</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>364</v>
+        <v>466</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
@@ -4157,7 +4388,7 @@
         <v>252</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>364</v>
+        <v>462</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.3">
@@ -4165,7 +4396,7 @@
         <v>253</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>364</v>
+        <v>467</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.3">
@@ -4173,7 +4404,7 @@
         <v>254</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>364</v>
+        <v>468</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.3">
@@ -4181,7 +4412,7 @@
         <v>255</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.3">
@@ -4189,7 +4420,7 @@
         <v>256</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.3">
@@ -4205,7 +4436,7 @@
         <v>258</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.3">
@@ -4213,7 +4444,7 @@
         <v>259</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.3">
@@ -4221,7 +4452,7 @@
         <v>260</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.3">
@@ -4237,7 +4468,7 @@
         <v>262</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.3">
@@ -4253,7 +4484,7 @@
         <v>264</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.3">
@@ -4261,7 +4492,7 @@
         <v>265</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.3">
@@ -4269,7 +4500,7 @@
         <v>266</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.3">
@@ -4277,7 +4508,7 @@
         <v>267</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.3">
@@ -4293,7 +4524,7 @@
         <v>269</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.3">
@@ -4309,7 +4540,7 @@
         <v>271</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.3">
@@ -4325,7 +4556,7 @@
         <v>273</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.3">
@@ -4341,7 +4572,7 @@
         <v>275</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.3">
@@ -4354,15 +4585,15 @@
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A279" s="3" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A280" s="3" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="B280" s="3" t="s">
         <v>279</v>
@@ -4370,15 +4601,15 @@
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A281" s="3" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A282" s="3" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="B282" s="3" t="s">
         <v>279</v>
@@ -4386,15 +4617,15 @@
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A283" s="3" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A284" s="3" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="B284" s="3" t="s">
         <v>279</v>
@@ -4402,15 +4633,15 @@
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A285" s="3" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A286" s="3" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="B286" s="3" t="s">
         <v>279</v>
@@ -4418,15 +4649,15 @@
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A287" s="3" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A288" s="3" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="B288" s="3" t="s">
         <v>279</v>
@@ -4434,15 +4665,15 @@
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A289" s="3" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A290" s="3" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="B290" s="3" t="s">
         <v>279</v>
@@ -4450,15 +4681,15 @@
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A291" s="3" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A292" s="3" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="B292" s="3" t="s">
         <v>279</v>

</xml_diff>